<commit_message>
minor correction to visit6
</commit_message>
<xml_diff>
--- a/Barcoding/excel.xlsx
+++ b/Barcoding/excel.xlsx
@@ -340,7 +340,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -354,197 +354,10 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>A001.V4.15</t>
+          <t>I001.V6- -</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>A001.V4.15</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>A001.V4.15</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>A001.V4.15</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>A001.V4.15</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>A001.V4.15</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
-      <c r="A8" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
-      <c r="A9" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>2021</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>food@</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>A001.V4.16</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
         <is>
           <t>2021</t>
         </is>

</xml_diff>